<commit_message>
updates to README and tracker
</commit_message>
<xml_diff>
--- a/schedule/tracker.xlsx
+++ b/schedule/tracker.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koer2434/Documents/eagle/projects/open_covg_daq_pcb/schedule/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A978FE44-941C-484D-9419-91E8728F693C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9627CC2C-515A-EB4F-B1C2-952CC1DC32C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{915DFBD2-32D0-0A46-9CC1-E54BC8CB7CA5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15600" windowHeight="21140" xr2:uid="{915DFBD2-32D0-0A46-9CC1-E54BC8CB7CA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -483,7 +483,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>